<commit_message>
Dodany opis wykresów + formatowanie
</commit_message>
<xml_diff>
--- a/Benchmarks-results/Prometheus/całka wykresy/całka - summary.xlsx
+++ b/Benchmarks-results/Prometheus/całka wykresy/całka - summary.xlsx
@@ -65,7 +65,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -105,16 +105,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -3510,25 +3510,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="98276864"/>
-        <c:axId val="98278400"/>
+        <c:axId val="115677056"/>
+        <c:axId val="115678592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98276864"/>
+        <c:axId val="115677056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98278400"/>
+        <c:crossAx val="115678592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98278400"/>
+        <c:axId val="115678592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3536,7 +3536,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98276864"/>
+        <c:crossAx val="115677056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3549,7 +3549,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3644,7 +3644,7 @@
             <c:numRef>
               <c:f>Arkusz1!$E$16:$E$27</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>132.51903302400001</c:v>
@@ -3699,7 +3699,7 @@
             <c:numRef>
               <c:f>Arkusz1!$E$32:$E$43</c:f>
               <c:numCache>
-                <c:formatCode>0.000000000</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>135.67784548200001</c:v>
@@ -3742,33 +3742,33 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="99350016"/>
-        <c:axId val="99361920"/>
+        <c:axId val="115724672"/>
+        <c:axId val="115726208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99350016"/>
+        <c:axId val="115724672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99361920"/>
+        <c:crossAx val="115726208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99361920"/>
+        <c:axId val="115726208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99350016"/>
+        <c:crossAx val="115724672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3781,7 +3781,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3861,7 +3861,7 @@
             <c:numRef>
               <c:f>Arkusz1!$E$5:$E$10</c:f>
               <c:numCache>
-                <c:formatCode>0.000000000</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>2353.8342543240001</c:v>
@@ -3886,33 +3886,33 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="131317120"/>
-        <c:axId val="131470080"/>
+        <c:axId val="117843456"/>
+        <c:axId val="117844992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="131317120"/>
+        <c:axId val="117843456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131470080"/>
+        <c:crossAx val="117844992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131470080"/>
+        <c:axId val="117844992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.000000000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131317120"/>
+        <c:crossAx val="117843456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3925,7 +3925,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3975,7 +3975,7 @@
             <c:numRef>
               <c:f>Arkusz1!$E$16:$E$27</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>132.51903302400001</c:v>
@@ -4063,25 +4063,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="115514752"/>
-        <c:axId val="115677824"/>
+        <c:axId val="117877376"/>
+        <c:axId val="117883264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115514752"/>
+        <c:axId val="117877376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115677824"/>
+        <c:crossAx val="117883264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115677824"/>
+        <c:axId val="117883264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4089,7 +4089,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115514752"/>
+        <c:crossAx val="117877376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4102,7 +4102,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4147,7 +4147,7 @@
             <c:numRef>
               <c:f>Arkusz1!$E$32:$E$43</c:f>
               <c:numCache>
-                <c:formatCode>0.000000000</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>135.67784548200001</c:v>
@@ -4247,7 +4247,7 @@
             <c:numRef>
               <c:f>Arkusz1!$E$32:$E$43</c:f>
               <c:numCache>
-                <c:formatCode>0.000000000</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>135.67784548200001</c:v>
@@ -4335,25 +4335,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="130781184"/>
-        <c:axId val="164386688"/>
+        <c:axId val="122172160"/>
+        <c:axId val="122173696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="130781184"/>
+        <c:axId val="122172160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="0.000000000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164386688"/>
+        <c:crossAx val="122173696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="164386688"/>
+        <c:axId val="122173696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4361,7 +4361,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130781184"/>
+        <c:crossAx val="122172160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4374,7 +4374,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4424,7 +4424,7 @@
             <c:numRef>
               <c:f>Arkusz1!$E$5:$E$10</c:f>
               <c:numCache>
-                <c:formatCode>0.000000000</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>2353.8342543240001</c:v>
@@ -4476,25 +4476,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133129728"/>
-        <c:axId val="133131264"/>
+        <c:axId val="122185600"/>
+        <c:axId val="122187136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133129728"/>
+        <c:axId val="122185600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="0.000000000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133131264"/>
+        <c:crossAx val="122187136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133131264"/>
+        <c:axId val="122187136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4502,7 +4502,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133129728"/>
+        <c:crossAx val="122185600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4515,7 +4515,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4616,15 +4616,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4645,15 +4645,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1371599</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7306,8 +7306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7332,7 +7332,7 @@
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -7343,7 +7343,7 @@
       <c r="D5" s="2">
         <v>8388608</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="6">
         <v>2353.8342543240001</v>
       </c>
       <c r="F5" s="2">
@@ -7358,7 +7358,7 @@
       <c r="D6" s="2">
         <v>4194304</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="6">
         <v>580.40452105099996</v>
       </c>
       <c r="F6" s="2">
@@ -7373,7 +7373,7 @@
       <c r="D7" s="2">
         <v>2097152</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="6">
         <v>145.50123349899999</v>
       </c>
       <c r="F7" s="2">
@@ -7388,7 +7388,7 @@
       <c r="D8" s="2">
         <v>1048576</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="6">
         <v>37.104339269</v>
       </c>
       <c r="F8" s="2">
@@ -7403,7 +7403,7 @@
       <c r="D9" s="2">
         <v>524288</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="6">
         <v>10.402122986</v>
       </c>
       <c r="F9" s="2">
@@ -7418,7 +7418,7 @@
       <c r="D10" s="2">
         <v>262144</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="6">
         <v>2.702683242</v>
       </c>
       <c r="F10" s="2">
@@ -7470,10 +7470,10 @@
       </c>
     </row>
     <row r="16" spans="4:7">
-      <c r="D16" s="6">
+      <c r="D16" s="4">
         <v>536870912</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="6">
         <v>132.51903302400001</v>
       </c>
       <c r="F16" s="2">
@@ -7487,7 +7487,7 @@
       <c r="D17" s="2">
         <v>268435456</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="6">
         <v>66.600740545999997</v>
       </c>
       <c r="F17" s="2">
@@ -7501,7 +7501,7 @@
       <c r="D18" s="2">
         <v>134217728</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="6">
         <v>33.646701516</v>
       </c>
       <c r="F18" s="2">
@@ -7515,7 +7515,7 @@
       <c r="D19" s="2">
         <v>67108864</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="6">
         <v>17.166549789000001</v>
       </c>
       <c r="F19" s="2">
@@ -7529,7 +7529,7 @@
       <c r="D20" s="2">
         <v>33554432</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="6">
         <v>11.306908883</v>
       </c>
       <c r="F20" s="2">
@@ -7543,7 +7543,7 @@
       <c r="D21" s="2">
         <v>16777216</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="6">
         <v>11.148561609</v>
       </c>
       <c r="F21" s="2">
@@ -7557,7 +7557,7 @@
       <c r="D22" s="2">
         <v>8388608</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="6">
         <v>11.010391404</v>
       </c>
       <c r="F22" s="2">
@@ -7571,7 +7571,7 @@
       <c r="D23" s="2">
         <v>4194304</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="6">
         <v>11.039786851000001</v>
       </c>
       <c r="F23" s="2">
@@ -7585,7 +7585,7 @@
       <c r="D24" s="2">
         <v>2097152</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="6">
         <v>10.963811723999999</v>
       </c>
       <c r="F24" s="2">
@@ -7599,7 +7599,7 @@
       <c r="D25" s="2">
         <v>1048576</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="6">
         <v>11.010572836</v>
       </c>
       <c r="F25" s="2">
@@ -7613,7 +7613,7 @@
       <c r="D26" s="2">
         <v>524288</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="6">
         <v>11.003288191999999</v>
       </c>
       <c r="F26" s="2">
@@ -7627,7 +7627,7 @@
       <c r="D27" s="2">
         <v>262144</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="6">
         <v>10.965948655</v>
       </c>
       <c r="F27" s="2">
@@ -7666,7 +7666,7 @@
       <c r="D32" s="2">
         <v>536870912</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="5">
         <v>135.67784548200001</v>
       </c>
       <c r="F32" s="2">
@@ -7686,7 +7686,7 @@
       <c r="D33" s="2">
         <v>268435456</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="6">
         <v>68.053597839999995</v>
       </c>
       <c r="F33" s="2">
@@ -7706,7 +7706,7 @@
       <c r="D34" s="2">
         <v>134217728</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="6">
         <v>34.275135929000001</v>
       </c>
       <c r="F34" s="2">
@@ -7726,7 +7726,7 @@
       <c r="D35" s="2">
         <v>67108864</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="6">
         <v>17.402544657</v>
       </c>
       <c r="F35" s="2">
@@ -7746,7 +7746,7 @@
       <c r="D36" s="2">
         <v>33554432</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="6">
         <v>9.004032445</v>
       </c>
       <c r="F36" s="2">
@@ -7766,7 +7766,7 @@
       <c r="D37" s="2">
         <v>16777216</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="6">
         <v>5.887043791</v>
       </c>
       <c r="F37" s="2">
@@ -7786,7 +7786,7 @@
       <c r="D38" s="2">
         <v>8388608</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="6">
         <v>5.8310847900000002</v>
       </c>
       <c r="F38" s="2">
@@ -7806,7 +7806,7 @@
       <c r="D39" s="2">
         <v>4194304</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="6">
         <v>5.8298811649999998</v>
       </c>
       <c r="F39" s="2">
@@ -7826,7 +7826,7 @@
       <c r="D40" s="2">
         <v>2097152</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="6">
         <v>5.8007926789999997</v>
       </c>
       <c r="F40" s="2">
@@ -7846,7 +7846,7 @@
       <c r="D41" s="2">
         <v>1048576</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="6">
         <v>5.7904401529999996</v>
       </c>
       <c r="F41" s="2">
@@ -7866,7 +7866,7 @@
       <c r="D42" s="2">
         <v>524288</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="6">
         <v>5.8059270950000004</v>
       </c>
       <c r="F42" s="2">
@@ -7886,7 +7886,7 @@
       <c r="D43" s="2">
         <v>262144</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="6">
         <v>5.8193430800000003</v>
       </c>
       <c r="F43" s="2">

</xml_diff>

<commit_message>
Dodane poprawne wykresy - brak opisów i wniosków
</commit_message>
<xml_diff>
--- a/Benchmarks-results/Prometheus/całka wykresy/całka - summary.xlsx
+++ b/Benchmarks-results/Prometheus/całka wykresy/całka - summary.xlsx
@@ -65,7 +65,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -111,10 +111,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -3510,25 +3510,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="115677056"/>
-        <c:axId val="115678592"/>
+        <c:axId val="116922240"/>
+        <c:axId val="116923776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115677056"/>
+        <c:axId val="116922240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115678592"/>
+        <c:crossAx val="116923776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115678592"/>
+        <c:axId val="116923776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3536,7 +3536,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115677056"/>
+        <c:crossAx val="116922240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3549,7 +3549,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3742,25 +3742,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="115724672"/>
-        <c:axId val="115726208"/>
+        <c:axId val="116969856"/>
+        <c:axId val="116971392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115724672"/>
+        <c:axId val="116969856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115726208"/>
+        <c:crossAx val="116971392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115726208"/>
+        <c:axId val="116971392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3768,7 +3768,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115724672"/>
+        <c:crossAx val="116969856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3781,7 +3781,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3886,25 +3886,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="117843456"/>
-        <c:axId val="117844992"/>
+        <c:axId val="117315072"/>
+        <c:axId val="117316608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="117843456"/>
+        <c:axId val="117315072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117844992"/>
+        <c:crossAx val="117316608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117844992"/>
+        <c:axId val="117316608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3912,7 +3912,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117843456"/>
+        <c:crossAx val="117315072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3925,7 +3925,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4063,25 +4063,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="117877376"/>
-        <c:axId val="117883264"/>
+        <c:axId val="117348992"/>
+        <c:axId val="117363072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="117877376"/>
+        <c:axId val="117348992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117883264"/>
+        <c:crossAx val="117363072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117883264"/>
+        <c:axId val="117363072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4089,7 +4089,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117877376"/>
+        <c:crossAx val="117348992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4102,7 +4102,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4132,18 +4132,15 @@
     </c:title>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>Energia - karta 1 [J]</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Arkusz1!$E$32:$E$43</c:f>
               <c:numCache>
@@ -4187,8 +4184,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Arkusz1!$H$32:$H$43</c:f>
               <c:numCache>
@@ -4232,7 +4229,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4240,10 +4238,7 @@
           <c:tx>
             <c:v>Energia - karta 2 [J]</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Arkusz1!$E$32:$E$43</c:f>
               <c:numCache>
@@ -4287,8 +4282,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Arkusz1!$I$32:$I$43</c:f>
               <c:numCache>
@@ -4332,28 +4327,26 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="122172160"/>
-        <c:axId val="122173696"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="122172160"/>
+        <c:axId val="149135744"/>
+        <c:axId val="117451008"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="149135744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122173696"/>
+        <c:crossAx val="117451008"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="122173696"/>
+        <c:axId val="117451008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4361,9 +4354,9 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122172160"/>
+        <c:crossAx val="149135744"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4374,7 +4367,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4476,25 +4469,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="122185600"/>
-        <c:axId val="122187136"/>
+        <c:axId val="117467008"/>
+        <c:axId val="117468544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122185600"/>
+        <c:axId val="117467008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122187136"/>
+        <c:crossAx val="117468544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122187136"/>
+        <c:axId val="117468544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4502,7 +4495,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122185600"/>
+        <c:crossAx val="117467008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4515,7 +4508,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7306,8 +7299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>